<commit_message>
added project status to the report
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/default.xlsx
+++ b/Base/src/main/resources/templates/default.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="287">
   <si>
     <t xml:space="preserve"># of Users </t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total Hours </t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1146,6 +1149,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1466,12 +1470,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,30 +1485,31 @@
     <col min="3" max="3" width="8.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="44" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="5" spans="1:10">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="5" spans="1:11">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1512,11 +1517,12 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -1533,77 +1539,82 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7"/>
+      <c r="F7" s="21"/>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="J7"/>
+      <c r="I7"/>
+      <c r="K7"/>
     </row>
-    <row r="8" spans="1:10" ht="17.45" customHeight="1">
-      <c r="J8" s="18" t="s">
+    <row r="8" spans="1:11" ht="17.45" customHeight="1">
+      <c r="K8" s="18" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="19" customFormat="1" ht="17.45" customHeight="1">
+    <row r="9" spans="1:11" s="19" customFormat="1" ht="17.45" customHeight="1">
       <c r="A9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="2"/>
+      <c r="K9" s="18" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="F10" s="20" t="s">
+    <row r="10" spans="1:11">
+      <c r="G10" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="K10" s="18" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="J11" s="18" t="s">
+    <row r="11" spans="1:11">
+      <c r="K11" s="18" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="J12" s="17" t="s">
+    <row r="12" spans="1:11">
+      <c r="K12" s="17" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="J13" s="18" t="s">
+    <row r="13" spans="1:11">
+      <c r="K13" s="18" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="J14" s="18" t="s">
+    <row r="14" spans="1:11">
+      <c r="K14" s="18" t="s">
         <v>285</v>
       </c>
     </row>
@@ -1627,151 +1638,151 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:88">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="21" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="21" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="21" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="21" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="21" t="s">
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="21" t="s">
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="21" t="s">
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-      <c r="AC3" s="21" t="s">
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="21" t="s">
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="21" t="s">
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="21" t="s">
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="21" t="s">
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AP3" s="22"/>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="21" t="s">
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="21" t="s">
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AV3" s="22"/>
-      <c r="AW3" s="22"/>
-      <c r="AX3" s="21" t="s">
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AY3" s="22"/>
-      <c r="AZ3" s="22"/>
-      <c r="BA3" s="21" t="s">
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="BB3" s="22"/>
-      <c r="BC3" s="22"/>
-      <c r="BD3" s="21" t="s">
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="BE3" s="22"/>
-      <c r="BF3" s="22"/>
-      <c r="BG3" s="21" t="s">
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="BH3" s="22"/>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="21" t="s">
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BK3" s="22"/>
-      <c r="BL3" s="22"/>
-      <c r="BM3" s="21" t="s">
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BN3" s="22"/>
-      <c r="BO3" s="22"/>
-      <c r="BP3" s="21" t="s">
+      <c r="BN3" s="23"/>
+      <c r="BO3" s="23"/>
+      <c r="BP3" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="BQ3" s="22"/>
-      <c r="BR3" s="22"/>
-      <c r="BS3" s="21" t="s">
+      <c r="BQ3" s="23"/>
+      <c r="BR3" s="23"/>
+      <c r="BS3" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="BT3" s="22"/>
-      <c r="BU3" s="22"/>
-      <c r="BV3" s="21" t="s">
+      <c r="BT3" s="23"/>
+      <c r="BU3" s="23"/>
+      <c r="BV3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="BW3" s="22"/>
-      <c r="BX3" s="22"/>
-      <c r="BY3" s="21" t="s">
+      <c r="BW3" s="23"/>
+      <c r="BX3" s="23"/>
+      <c r="BY3" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="BZ3" s="22"/>
-      <c r="CA3" s="22"/>
-      <c r="CB3" s="21" t="s">
+      <c r="BZ3" s="23"/>
+      <c r="CA3" s="23"/>
+      <c r="CB3" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="CC3" s="22"/>
-      <c r="CD3" s="22"/>
-      <c r="CE3" s="21" t="s">
+      <c r="CC3" s="23"/>
+      <c r="CD3" s="23"/>
+      <c r="CE3" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="CF3" s="22"/>
-      <c r="CG3" s="22"/>
-      <c r="CH3" s="21" t="s">
+      <c r="CF3" s="23"/>
+      <c r="CG3" s="23"/>
+      <c r="CH3" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="CI3" s="22"/>
-      <c r="CJ3" s="22"/>
+      <c r="CI3" s="23"/>
+      <c r="CJ3" s="23"/>
     </row>
     <row r="4" spans="1:88">
       <c r="A4" s="11" t="s">
@@ -8425,6 +8436,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AU3:AW3"/>
+    <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="BA3:BC3"/>
+    <mergeCell ref="BD3:BF3"/>
+    <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="BY3:CA3"/>
     <mergeCell ref="CB3:CD3"/>
     <mergeCell ref="CE3:CG3"/>
@@ -8434,26 +8465,6 @@
     <mergeCell ref="BP3:BR3"/>
     <mergeCell ref="BS3:BU3"/>
     <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="AU3:AW3"/>
-    <mergeCell ref="AX3:AZ3"/>
-    <mergeCell ref="BA3:BC3"/>
-    <mergeCell ref="BD3:BF3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Project Reporting - Total hours should be excluding Public holidays and leaves. However it is only excluding Public holidays now. This will give incorrect utilization % Project Reporting - Project total hours at row level is not adding the last column/employ. Formula range is starting from Task name column only so it is missing out last column
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/default.xlsx
+++ b/Base/src/main/resources/templates/default.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Workspace-famstack\bops\Base\src\main\resources\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="Reporting" sheetId="1" r:id="rId1"/>
     <sheet name="Emp Utilization" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -853,9 +849,6 @@
     <t>NON_BILLABLE</t>
   </si>
   <si>
-    <t>Total Hours</t>
-  </si>
-  <si>
     <t>Utilization</t>
   </si>
   <si>
@@ -884,6 +877,9 @@
   </si>
   <si>
     <t>Project Category</t>
+  </si>
+  <si>
+    <t>Total Task Hours</t>
   </si>
 </sst>
 </file>
@@ -1476,10 +1472,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1545,13 +1541,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>287</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>6</v>
@@ -1563,7 +1559,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1581,7 +1577,7 @@
     <row r="8" spans="1:12" ht="17.45" customHeight="1">
       <c r="K8" s="18"/>
       <c r="L8" s="18" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="19" customFormat="1" ht="17.45" customHeight="1">
@@ -1599,7 +1595,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1608,31 +1604,31 @@
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="K11" s="18"/>
       <c r="L11" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="K13" s="18"/>
       <c r="L13" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="K14" s="18"/>
       <c r="L14" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -8453,6 +8449,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AU3:AW3"/>
+    <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="BA3:BC3"/>
+    <mergeCell ref="BD3:BF3"/>
+    <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="BY3:CA3"/>
     <mergeCell ref="CB3:CD3"/>
     <mergeCell ref="CE3:CG3"/>
@@ -8462,26 +8478,6 @@
     <mergeCell ref="BP3:BR3"/>
     <mergeCell ref="BS3:BU3"/>
     <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="AU3:AW3"/>
-    <mergeCell ref="AX3:AZ3"/>
-    <mergeCell ref="BA3:BC3"/>
-    <mergeCell ref="BD3:BF3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
static data reporting enabled for some of the team
</commit_message>
<xml_diff>
--- a/Base/src/main/resources/templates/default.xlsx
+++ b/Base/src/main/resources/templates/default.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="281">
   <si>
     <t xml:space="preserve"># of Users </t>
   </si>
@@ -850,27 +850,6 @@
     <t>02:27</t>
   </si>
   <si>
-    <t>NON_BILLABLE</t>
-  </si>
-  <si>
-    <t>Utilization</t>
-  </si>
-  <si>
-    <t>Leave Hours</t>
-  </si>
-  <si>
-    <t>Public Holiday hours</t>
-  </si>
-  <si>
-    <t>Excess Working Hours</t>
-  </si>
-  <si>
-    <t>Total Hours available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Hours </t>
-  </si>
-  <si>
     <t>Task Name</t>
   </si>
   <si>
@@ -881,9 +860,6 @@
   </si>
   <si>
     <t>Project Category</t>
-  </si>
-  <si>
-    <t>Total Task Hours</t>
   </si>
   <si>
     <t>Account</t>
@@ -1102,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1148,14 +1124,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1478,12 +1446,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1551,16 +1519,16 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>6</v>
@@ -1572,7 +1540,7 @@
         <v>8</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1580,71 +1548,13 @@
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="17"/>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="I7" s="23"/>
+      <c r="I7" s="19"/>
       <c r="J7"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" ht="17.45" customHeight="1">
-      <c r="L8" s="18"/>
-      <c r="M8" s="18" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="19" customFormat="1" ht="17.45" customHeight="1">
-      <c r="A9"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="G10" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="L11" s="18"/>
-      <c r="M11" s="18" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="L12" s="17"/>
-      <c r="M12" s="17" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="L13" s="18"/>
-      <c r="M13" s="18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="L14" s="18"/>
-      <c r="M14" s="18" t="s">
-        <v>282</v>
-      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1666,151 +1576,151 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:88">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="24" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="24" t="s">
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24" t="s">
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="24" t="s">
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="24" t="s">
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="24" t="s">
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="24" t="s">
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="24" t="s">
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="24" t="s">
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="24" t="s">
+      <c r="AM3" s="21"/>
+      <c r="AN3" s="21"/>
+      <c r="AO3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="24" t="s">
+      <c r="AP3" s="21"/>
+      <c r="AQ3" s="21"/>
+      <c r="AR3" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="24" t="s">
+      <c r="AS3" s="21"/>
+      <c r="AT3" s="21"/>
+      <c r="AU3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="24" t="s">
+      <c r="AV3" s="21"/>
+      <c r="AW3" s="21"/>
+      <c r="AX3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="AY3" s="25"/>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="24" t="s">
+      <c r="AY3" s="21"/>
+      <c r="AZ3" s="21"/>
+      <c r="BA3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="24" t="s">
+      <c r="BB3" s="21"/>
+      <c r="BC3" s="21"/>
+      <c r="BD3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="BE3" s="25"/>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="24" t="s">
+      <c r="BE3" s="21"/>
+      <c r="BF3" s="21"/>
+      <c r="BG3" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="BH3" s="25"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="24" t="s">
+      <c r="BH3" s="21"/>
+      <c r="BI3" s="21"/>
+      <c r="BJ3" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="24" t="s">
+      <c r="BK3" s="21"/>
+      <c r="BL3" s="21"/>
+      <c r="BM3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BN3" s="25"/>
-      <c r="BO3" s="25"/>
-      <c r="BP3" s="24" t="s">
+      <c r="BN3" s="21"/>
+      <c r="BO3" s="21"/>
+      <c r="BP3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="24" t="s">
+      <c r="BQ3" s="21"/>
+      <c r="BR3" s="21"/>
+      <c r="BS3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="24" t="s">
+      <c r="BT3" s="21"/>
+      <c r="BU3" s="21"/>
+      <c r="BV3" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="24" t="s">
+      <c r="BW3" s="21"/>
+      <c r="BX3" s="21"/>
+      <c r="BY3" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="24" t="s">
+      <c r="BZ3" s="21"/>
+      <c r="CA3" s="21"/>
+      <c r="CB3" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="CC3" s="25"/>
-      <c r="CD3" s="25"/>
-      <c r="CE3" s="24" t="s">
+      <c r="CC3" s="21"/>
+      <c r="CD3" s="21"/>
+      <c r="CE3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="CF3" s="25"/>
-      <c r="CG3" s="25"/>
-      <c r="CH3" s="24" t="s">
+      <c r="CF3" s="21"/>
+      <c r="CG3" s="21"/>
+      <c r="CH3" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="CI3" s="25"/>
-      <c r="CJ3" s="25"/>
+      <c r="CI3" s="21"/>
+      <c r="CJ3" s="21"/>
     </row>
     <row r="4" spans="1:88">
       <c r="A4" s="11" t="s">
@@ -8464,6 +8374,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AU3:AW3"/>
+    <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="BA3:BC3"/>
+    <mergeCell ref="BD3:BF3"/>
+    <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="BY3:CA3"/>
     <mergeCell ref="CB3:CD3"/>
     <mergeCell ref="CE3:CG3"/>
@@ -8473,26 +8403,6 @@
     <mergeCell ref="BP3:BR3"/>
     <mergeCell ref="BS3:BU3"/>
     <mergeCell ref="BV3:BX3"/>
-    <mergeCell ref="AU3:AW3"/>
-    <mergeCell ref="AX3:AZ3"/>
-    <mergeCell ref="BA3:BC3"/>
-    <mergeCell ref="BD3:BF3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>